<commit_message>
Mudei Estilos e imagens
</commit_message>
<xml_diff>
--- a/db/Produtos.xlsx
+++ b/db/Produtos.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="4005" windowWidth="19440" windowHeight="12210"/>
+    <workbookView xWindow="5955" yWindow="4005" windowWidth="19440" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Monitores" sheetId="2" r:id="rId1"/>
-    <sheet name="Placas Gráficas" sheetId="1" r:id="rId2"/>
-    <sheet name="Caixas" sheetId="3" r:id="rId3"/>
+    <sheet name="T-Shirt" sheetId="2" r:id="rId1"/>
+    <sheet name="Chuteiras Futebol" sheetId="1" r:id="rId2"/>
+    <sheet name="T-Shirt Futebol" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -23,20 +23,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
   <si>
     <t>Código</t>
   </si>
   <si>
-    <t>Designação</t>
-  </si>
-  <si>
     <t>Preço</t>
   </si>
   <si>
-    <t>Quantidade</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -76,132 +70,15 @@
     <t>Marca</t>
   </si>
   <si>
-    <t>nvidia</t>
-  </si>
-  <si>
-    <t>amd</t>
-  </si>
-  <si>
     <t>Fabricante</t>
   </si>
   <si>
-    <t>ASUS</t>
-  </si>
-  <si>
-    <t>MSI</t>
-  </si>
-  <si>
-    <t>Gigabyte</t>
-  </si>
-  <si>
-    <t>EVGA</t>
-  </si>
-  <si>
-    <t>Palit</t>
-  </si>
-  <si>
-    <t>Sapphire</t>
-  </si>
-  <si>
-    <t>RTX 2060</t>
-  </si>
-  <si>
-    <t>RTX 2070</t>
-  </si>
-  <si>
-    <t>RTX 2080</t>
-  </si>
-  <si>
-    <t>GTX 1660 TI</t>
-  </si>
-  <si>
-    <t>GTX 1070</t>
-  </si>
-  <si>
-    <t>GT 1030</t>
-  </si>
-  <si>
-    <t>TITAN</t>
-  </si>
-  <si>
-    <t>GTS 210</t>
-  </si>
-  <si>
-    <t>Vega 56</t>
-  </si>
-  <si>
-    <t>Vega 64</t>
-  </si>
-  <si>
-    <t>RX 550</t>
-  </si>
-  <si>
-    <t>RX 590</t>
-  </si>
-  <si>
-    <t>Asus</t>
-  </si>
-  <si>
-    <t>AOC</t>
-  </si>
-  <si>
     <t>Sku</t>
   </si>
   <si>
     <t>Nome</t>
   </si>
   <si>
-    <t>Antec ISK 300-150 EC PC 150W Preto caixa para computador</t>
-  </si>
-  <si>
-    <t>Cooler Master CM 690 III Torre-Midi Preto caixa para computador</t>
-  </si>
-  <si>
-    <t>UNYKA - CAIXA DESKTOP SLIM M.ATX UK-2007 USB 3.0 400W PRETA</t>
-  </si>
-  <si>
-    <t>UNYKAch Blast Ice Torre Preto, Branco caixa para computador</t>
-  </si>
-  <si>
-    <t>ASUS - PC VIVOPC I5-7200U S/MEN S/ HD S/SO - UN65U-BM009M</t>
-  </si>
-  <si>
-    <t>MARS GAMING - BUNDLE - MARS GAMING - CAIXA MC0 VENTOINHA MF12G</t>
-  </si>
-  <si>
-    <t>ASUS UN65H-M227M BGA 1356 2.3GHz i3-6100U PC de 0,88L Azul</t>
-  </si>
-  <si>
-    <t>ASUS UN65U-BM008M BGA 1356 2.40GHz i3-7100U Azul</t>
-  </si>
-  <si>
-    <t>COOLER MASTER - MASTER ATX MASTERCASE MAKER 5T PRETA SEM FONTE</t>
-  </si>
-  <si>
-    <t>NOX - Ark Gaming case</t>
-  </si>
-  <si>
-    <t>Aerocool BATTLEHAWK Torre-Midi Preto caixa para computador</t>
-  </si>
-  <si>
-    <t>Aerocool AERO800 Torre-Midi Cinzento, Preto caixa para computador</t>
-  </si>
-  <si>
-    <t>Aerocool AERO800 Torre-Midi Preto, Branco caixa para computador</t>
-  </si>
-  <si>
-    <t>Aerocool VS-1 Midi Tower Case - Black Torre-Midi Preto caixa para computador</t>
-  </si>
-  <si>
-    <t>Aerocool VS3 Advance Torre-Midi Preto caixa para computador</t>
-  </si>
-  <si>
-    <t>Aerocool V3X Advance Torre-Midi Preto caixa para computador</t>
-  </si>
-  <si>
-    <t>Tacens AC017AD Mini-Torre Preto caixa para computador</t>
-  </si>
-  <si>
     <t>13</t>
   </si>
   <si>
@@ -220,34 +97,118 @@
     <t>18</t>
   </si>
   <si>
-    <t>Laranja-Lima</t>
-  </si>
-  <si>
     <t>Preço /Kg</t>
   </si>
   <si>
-    <t>Morango Amahou</t>
-  </si>
-  <si>
-    <t>Melancia</t>
-  </si>
-  <si>
-    <t>Maça Braeburn</t>
-  </si>
-  <si>
-    <t>Kiwi Gold</t>
-  </si>
-  <si>
-    <t>Banana da Madeira</t>
-  </si>
-  <si>
-    <t>Ananás</t>
-  </si>
-  <si>
-    <t>Limão</t>
-  </si>
-  <si>
-    <t>Abacate</t>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nike </t>
+  </si>
+  <si>
+    <t>Adidas</t>
+  </si>
+  <si>
+    <t>Vans</t>
+  </si>
+  <si>
+    <t>Fila</t>
+  </si>
+  <si>
+    <t>Supreme</t>
+  </si>
+  <si>
+    <t>Puma</t>
+  </si>
+  <si>
+    <t>T-Shirt Real Madrid</t>
+  </si>
+  <si>
+    <t>T-Shirt Barcelona</t>
+  </si>
+  <si>
+    <t>T-Shirt Bayern Munich</t>
+  </si>
+  <si>
+    <t>T-Shirt Manchester City</t>
+  </si>
+  <si>
+    <t>T-Shirt Marseille</t>
+  </si>
+  <si>
+    <t>T-Shirt Manchester United</t>
+  </si>
+  <si>
+    <t>T-Shirt Borussia Dortmund</t>
+  </si>
+  <si>
+    <t>T-Shirt Arsenal</t>
+  </si>
+  <si>
+    <t>T-Shirt AF Roma</t>
+  </si>
+  <si>
+    <t>T-Shirt Atletico De Madrid</t>
+  </si>
+  <si>
+    <t>T-Shirt Juventus</t>
+  </si>
+  <si>
+    <t>T-Shirt Ajax</t>
+  </si>
+  <si>
+    <t>T-Shirt Manchester United Second Equipment</t>
+  </si>
+  <si>
+    <t>T-Shirt Leicester City</t>
+  </si>
+  <si>
+    <t>T-Shirt FC Liverpool</t>
+  </si>
+  <si>
+    <t>T-Shirt PSG</t>
+  </si>
+  <si>
+    <t>T-Shirt Benfica</t>
+  </si>
+  <si>
+    <t>T-Shirt River Plate</t>
+  </si>
+  <si>
+    <t>Adidas Predator</t>
+  </si>
+  <si>
+    <t>Nike Hypervenom phantom</t>
+  </si>
+  <si>
+    <t>Nike Magista Obra Ii Ag-Pro</t>
+  </si>
+  <si>
+    <t> Nike Magista Obra II Pro FG</t>
+  </si>
+  <si>
+    <t>Nike Mercurial Superfly 360 Elite</t>
+  </si>
+  <si>
+    <t>Nike Mercurial Superfly VI </t>
+  </si>
+  <si>
+    <t>Nike Hypervenom</t>
+  </si>
+  <si>
+    <t>Nike Mercurial Victory VI NJR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adidas </t>
+  </si>
+  <si>
+    <t>Adidas JR VAPOR 12</t>
+  </si>
+  <si>
+    <t>Nike Hyper Venom 3 Preta</t>
+  </si>
+  <si>
+    <t>Nike Mercurial CR7</t>
   </si>
 </sst>
 </file>
@@ -257,7 +218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +232,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -294,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -308,17 +282,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
-      <alignment horizontal="center" vertical="bottom"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom"/>
@@ -343,11 +329,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela13" displayName="Tabela13" ref="A1:C13" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela13" displayName="Tabela13" ref="A1:C13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:C13"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Código" dataDxfId="2"/>
-    <tableColumn id="2" name="Nome" dataDxfId="0"/>
+    <tableColumn id="1" name="Código" dataDxfId="3"/>
+    <tableColumn id="2" name="Nome" dataDxfId="2"/>
     <tableColumn id="5" name="Preço /Kg" dataDxfId="1" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -355,14 +341,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F13" totalsRowShown="0">
-  <autoFilter ref="A1:F13"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D13" totalsRowShown="0">
+  <autoFilter ref="A1:D13"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Código"/>
-    <tableColumn id="3" name="Fabricante"/>
+    <tableColumn id="3" name="Fabricante" dataDxfId="0"/>
     <tableColumn id="4" name="Marca"/>
-    <tableColumn id="5" name="Designação"/>
-    <tableColumn id="7" name="Quantidade"/>
     <tableColumn id="6" name="Preço" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -658,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,142 +658,142 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="C2" s="5">
-        <v>1.0900000000000001</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="C3" s="5">
-        <v>2.58</v>
+        <v>10.99</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>1.79</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5">
-        <v>2.4900000000000002</v>
+        <v>10.99</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5">
-        <v>2.59</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5">
-        <v>2.99</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5">
-        <v>5.09</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5">
-        <v>1.69</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="C10" s="5">
-        <v>3.99</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5">
-        <v>310</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C12" s="5">
-        <v>150</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5">
-        <v>230</v>
+        <v>10.99</v>
       </c>
     </row>
   </sheetData>
@@ -822,286 +806,209 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="6">
+        <v>50.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6">
+        <v>80.989999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2">
+      <c r="B4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3" s="6">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4" s="6">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5" s="6">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6" s="6">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="B8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" s="6">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" s="6">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B10" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="6">
+        <v>89.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9" s="6">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="B11" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="6">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="B12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" s="6">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12">
-        <v>5</v>
-      </c>
-      <c r="F12" s="6">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
+      <c r="B13" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
-      </c>
-      <c r="F13" s="6">
-        <v>145</v>
+        <v>25</v>
+      </c>
+      <c r="D13" s="6">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1111,7 +1018,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,21 +1030,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C2" s="6">
         <v>94.99</v>
@@ -1145,120 +1052,120 @@
     </row>
     <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C3" s="6">
-        <v>102.99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C4" s="6">
-        <v>37.99</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C5" s="6">
-        <v>23.09</v>
+        <v>65.989999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C6" s="6">
-        <v>419.99</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6">
-        <v>94.99</v>
+        <v>50.99</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C8" s="6">
-        <v>21.19</v>
+        <v>49.99</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C9" s="6">
-        <v>391.99</v>
+        <v>40.99</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C10" s="6">
-        <v>350.99</v>
+        <v>49.99</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6">
-        <v>267.99</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C12" s="6">
-        <v>115.99</v>
+        <v>55.8</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6">
         <v>59.99</v>
@@ -1266,10 +1173,10 @@
     </row>
     <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C14" s="6">
         <v>69.989999999999995</v>
@@ -1277,32 +1184,32 @@
     </row>
     <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C15" s="6">
-        <v>78.989999999999995</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C16" s="6">
-        <v>37.79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6">
         <v>51.99</v>
@@ -1310,10 +1217,10 @@
     </row>
     <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C18" s="6">
         <v>37.19</v>
@@ -1321,10 +1228,10 @@
     </row>
     <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C19" s="6">
         <v>19.09</v>

</xml_diff>